<commit_message>
updates to PS schematic
</commit_message>
<xml_diff>
--- a/invoices/Parts_on_hand.xlsx
+++ b/invoices/Parts_on_hand.xlsx
@@ -1,19 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariscal\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25120" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="digi_order_4" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">digi_order_4!$A$1:$F$53</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
   <si>
     <t>Quantity</t>
   </si>
@@ -255,9 +253,6 @@
   </si>
   <si>
     <t>RELAY GEN PURPOSE SPST 30A 48V</t>
-  </si>
-  <si>
-    <t>1 CAMERON</t>
   </si>
   <si>
     <t>1N4004-TPMSCT-ND</t>
@@ -427,8 +422,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -909,8 +904,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1224,7 +1219,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1234,21 +1229,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1268,1047 +1263,1050 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2">
+        <v>1.68</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3">
+        <v>2.83</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4">
+        <v>22.34</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="F5">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>0.72</v>
-      </c>
-      <c r="F2">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>0.6</v>
-      </c>
-      <c r="F3">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
+      <c r="E7">
         <v>0.45</v>
       </c>
-      <c r="F4">
+      <c r="F7">
         <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>0.45</v>
-      </c>
-      <c r="F5">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>0.504</v>
-      </c>
-      <c r="F6">
-        <v>7.06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="F7">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="F8">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E8">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="F8">
-        <v>2.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
       <c r="E9">
-        <v>0.36</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="F9">
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>1.28</v>
+        <v>0.45</v>
       </c>
       <c r="F10">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="E11">
-        <v>1.593</v>
-      </c>
-      <c r="F11">
-        <v>19.12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="E12">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="F12">
-        <v>4.66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.247</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="E13">
-        <v>0.63</v>
-      </c>
-      <c r="F13">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6.43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>0.76</v>
+      </c>
+      <c r="F14">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="F15">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>0.41</v>
+      </c>
+      <c r="F16">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17">
+        <v>0.2316</v>
+      </c>
+      <c r="F17">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18">
+        <v>0.39</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>0.22</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14">
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="F14">
-        <v>2.78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15">
-        <v>5.7599999999999998E-2</v>
-      </c>
-      <c r="F15">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16">
-        <v>5.7599999999999998E-2</v>
-      </c>
-      <c r="F16">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
         <v>23</v>
       </c>
-      <c r="E17">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="F17">
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18">
-        <v>0.2</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19">
-        <v>0.76</v>
-      </c>
-      <c r="F19">
-        <v>3.04</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20">
-        <v>0.41</v>
-      </c>
-      <c r="F20">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
       <c r="E21">
-        <v>0.2316</v>
+        <v>1.28</v>
       </c>
       <c r="F21">
-        <v>5.79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E22">
+        <v>0.4</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
         <v>2</v>
       </c>
-      <c r="F22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>10</v>
-      </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E23">
-        <v>0.63</v>
-      </c>
-      <c r="F23">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.52</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E24">
-        <v>0.33700000000000002</v>
+        <v>0.52</v>
       </c>
       <c r="F24" s="1">
-        <v>5.39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25">
+        <v>0.24</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
         <v>64</v>
       </c>
-      <c r="E25">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F25" s="1">
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" t="s">
-        <v>67</v>
-      </c>
       <c r="E26">
-        <v>5.5E-2</v>
+        <v>0.41</v>
       </c>
       <c r="F26" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
         <v>64</v>
       </c>
       <c r="E27">
-        <v>22.34</v>
+        <v>0.34</v>
       </c>
       <c r="F27" s="1">
-        <v>44.68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28">
+        <v>2.42</v>
+      </c>
+      <c r="F28" s="2">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
         <v>10</v>
       </c>
-      <c r="B28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="F28" s="1">
-        <v>6.43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>12</v>
-      </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="E29">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2.87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.63</v>
+      </c>
+      <c r="F29">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="E30">
-        <v>3.05</v>
-      </c>
-      <c r="F30" s="1">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="F30">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E31">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="F31" s="1">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.63</v>
+      </c>
+      <c r="F31">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>0.72</v>
+      </c>
+      <c r="F32">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="F33">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <v>0.36</v>
+      </c>
+      <c r="F34">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
         <v>81</v>
       </c>
-      <c r="D32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32">
-        <v>0.247</v>
-      </c>
-      <c r="F32" s="1">
-        <v>2.4700000000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35">
+        <v>3.79</v>
+      </c>
+      <c r="F35" s="1">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36">
+        <v>1.593</v>
+      </c>
+      <c r="F36">
+        <v>19.12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33">
-        <v>3.79</v>
-      </c>
-      <c r="F33" s="1">
-        <v>7.58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37">
         <v>2</v>
       </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34">
-        <v>2.98</v>
-      </c>
-      <c r="F34" s="1">
-        <v>5.96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="F37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
         <v>1</v>
       </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35">
-        <v>3.05</v>
-      </c>
-      <c r="F35" s="1">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>10</v>
-      </c>
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36">
-        <v>0.255</v>
-      </c>
-      <c r="F36" s="1">
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>4</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37">
-        <v>0.24</v>
-      </c>
-      <c r="F37" s="1">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>8</v>
-      </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E38">
-        <v>0.47</v>
+        <v>1.91</v>
       </c>
       <c r="F38" s="1">
-        <v>3.76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E39">
-        <v>0.22</v>
+        <v>0.98</v>
       </c>
       <c r="F39" s="1">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="E40">
-        <v>0.4</v>
+        <v>3.58</v>
       </c>
       <c r="F40" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10.74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="E41">
-        <v>0.52</v>
+        <v>2.98</v>
       </c>
       <c r="F41" s="1">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E42">
-        <v>0.34</v>
+        <v>3.05</v>
       </c>
       <c r="F42" s="1">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
         <v>64</v>
       </c>
       <c r="E43">
-        <v>0.41</v>
+        <v>3.05</v>
       </c>
       <c r="F43" s="1">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>67</v>
       </c>
       <c r="E44">
-        <v>3.58</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F44" s="1">
-        <v>10.74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45">
+        <v>0.2</v>
+      </c>
+      <c r="F45">
         <v>2</v>
       </c>
-      <c r="B45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" t="s">
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>50</v>
+      </c>
+      <c r="B46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="F46">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="F48">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49">
+        <v>0.255</v>
+      </c>
+      <c r="F49" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50">
+        <v>0.47</v>
+      </c>
+      <c r="F50" s="1">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51">
+        <v>0.504</v>
+      </c>
+      <c r="F51">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
         <v>111</v>
       </c>
-      <c r="D45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45">
-        <v>0.52</v>
-      </c>
-      <c r="F45" s="1">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C52" t="s">
         <v>112</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D52" t="s">
         <v>113</v>
       </c>
-      <c r="D46" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46">
+      <c r="E52">
         <v>5.89</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F52" s="1">
         <v>5.89</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" t="s">
-        <v>116</v>
-      </c>
-      <c r="D47" t="s">
-        <v>23</v>
-      </c>
-      <c r="E47">
-        <v>0.98</v>
-      </c>
-      <c r="F47" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48">
-        <v>1.91</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>120</v>
-      </c>
-      <c r="C49" t="s">
-        <v>121</v>
-      </c>
-      <c r="D49" t="s">
-        <v>119</v>
-      </c>
-      <c r="E49">
-        <v>1.68</v>
-      </c>
-      <c r="F49" s="2">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="53" spans="1:6">
+      <c r="A53">
         <v>2</v>
       </c>
-      <c r="B50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" t="s">
-        <v>131</v>
-      </c>
-      <c r="E50">
-        <v>2.42</v>
-      </c>
-      <c r="F50" s="2">
-        <v>4.84</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
-        <v>124</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B53" t="s">
         <v>125</v>
       </c>
-      <c r="D51" t="s">
-        <v>119</v>
-      </c>
-      <c r="E51">
-        <v>2.83</v>
-      </c>
-      <c r="F51" s="2">
-        <v>2.83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>2</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C53" t="s">
         <v>126</v>
       </c>
-      <c r="C52" t="s">
-        <v>127</v>
-      </c>
-      <c r="D52" t="s">
-        <v>130</v>
-      </c>
-      <c r="E52">
+      <c r="D53" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53">
         <v>0.67</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F53" s="2">
         <v>1.34</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
-        <v>128</v>
-      </c>
-      <c r="C53" t="s">
-        <v>129</v>
-      </c>
-      <c r="D53" t="s">
-        <v>119</v>
-      </c>
-      <c r="E53">
-        <v>0.39</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0.39</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:F53">
+    <sortCondition ref="C1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
updates to PS, libary and Action items
</commit_message>
<xml_diff>
--- a/invoices/Parts_on_hand.xlsx
+++ b/invoices/Parts_on_hand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25120" windowHeight="14240"/>
+    <workbookView xWindow="-32020" yWindow="2240" windowWidth="25120" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="digi_order_4" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">digi_order_4!$A$1:$F$53</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -425,7 +425,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,6 +560,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -858,7 +874,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -901,13 +917,67 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="96">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -936,11 +1006,65 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1229,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2308,6 +2432,7 @@
     <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updates to PS schematic, created special 1N4004 part
</commit_message>
<xml_diff>
--- a/invoices/Parts_on_hand.xlsx
+++ b/invoices/Parts_on_hand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-29240" yWindow="1200" windowWidth="25120" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="digi_order_4" sheetId="1" r:id="rId1"/>
@@ -874,7 +874,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="102">
+  <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -977,13 +977,24 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="102">
+  <cellStyles count="112">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1042,6 +1053,11 @@
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1077,6 +1093,11 @@
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1355,7 +1376,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1365,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1766,7 +1787,7 @@
       <c r="B20" t="s">
         <v>77</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D20" t="s">

</xml_diff>

<commit_message>
finished powersuply :) updated parts on hand
</commit_message>
<xml_diff>
--- a/invoices/Parts_on_hand.xlsx
+++ b/invoices/Parts_on_hand.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="-28320" yWindow="500" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="digi_order_4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">digi_order_4!$A$1:$F$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">digi_order_4!$A$1:$E$64</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="155">
   <si>
     <t>Quantity</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Unit Price USD</t>
   </si>
   <si>
-    <t>Extended Price USD</t>
-  </si>
-  <si>
     <t>M10028-ND</t>
   </si>
   <si>
@@ -415,16 +412,87 @@
   </si>
   <si>
     <t xml:space="preserve">2 Carlos </t>
+  </si>
+  <si>
+    <t>493-7338-ND</t>
+  </si>
+  <si>
+    <t>CAP ALUM 330UF 20% 200V RADIAL</t>
+  </si>
+  <si>
+    <t>1 CAMERON</t>
+  </si>
+  <si>
+    <t>445-8517-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 50V X7R RADIAL</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>445-8348-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V X7R RADIAL</t>
+  </si>
+  <si>
+    <t>PPC330W-1CT-ND</t>
+  </si>
+  <si>
+    <t>RES 330 OHM 1W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>PPC33W-1CT-ND</t>
+  </si>
+  <si>
+    <t>RES 33 OHM 1W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>A105896CT-ND</t>
+  </si>
+  <si>
+    <t>RES 47.0K OHM 2W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>709-1020-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 500V X7R 0805</t>
+  </si>
+  <si>
+    <t>445-8441-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 100UF 6.3V X5R RADIAL</t>
+  </si>
+  <si>
+    <t>A33861-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER RT/A .100 4POS 15AU</t>
+  </si>
+  <si>
+    <t>A28401-ND</t>
+  </si>
+  <si>
+    <t>CONN RECPT 4POS .1" POL UNLOAD</t>
+  </si>
+  <si>
+    <t>1N5361BTPMSCT-ND</t>
+  </si>
+  <si>
+    <t>DIODE ZENER 5W 27V DO-15</t>
+  </si>
+  <si>
+    <t>FOR TEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -988,11 +1056,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="112">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1376,7 +1441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1384,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1396,11 +1461,10 @@
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1416,1048 +1480,1064 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
         <v>119</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2">
         <v>1.68</v>
       </c>
-      <c r="F2" s="2">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3">
         <v>2.83</v>
       </c>
-      <c r="F3" s="2">
-        <v>2.83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <v>22.34</v>
       </c>
-      <c r="F4" s="1">
-        <v>44.68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="E5">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="F5">
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
       <c r="E6">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="F6" s="1">
-        <v>5.39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="E7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8">
         <v>0.45</v>
       </c>
-      <c r="F7">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8">
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="F8">
-        <v>2.78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="F9">
-        <v>4.66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0.30599999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
         <v>0.45</v>
       </c>
-      <c r="F10">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2.87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12">
-        <v>0.247</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2.4700000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="C13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13">
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18">
         <v>0.64300000000000002</v>
       </c>
-      <c r="F13" s="1">
-        <v>6.43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D21" t="s">
         <v>49</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E21">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
         <v>50</v>
       </c>
-      <c r="E14">
-        <v>0.76</v>
-      </c>
-      <c r="F14">
-        <v>3.04</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="F15">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16">
-        <v>0.41</v>
-      </c>
-      <c r="F16">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C24" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D24" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17">
+      <c r="E24">
         <v>0.2316</v>
       </c>
-      <c r="F17">
-        <v>5.79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" t="s">
         <v>127</v>
       </c>
-      <c r="C18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18">
+      <c r="D25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25">
         <v>0.39</v>
       </c>
-      <c r="F18" s="2">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>0.22</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21">
-        <v>1.28</v>
-      </c>
-      <c r="F21">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22">
-        <v>0.4</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23">
-        <v>0.52</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>0.52</v>
-      </c>
-      <c r="F24" s="1">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25">
-        <v>0.24</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" t="s">
         <v>104</v>
       </c>
-      <c r="C26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26">
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34">
         <v>0.41</v>
       </c>
-      <c r="F26" s="1">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27">
-        <v>0.34</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" t="s">
-        <v>122</v>
-      </c>
-      <c r="D28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28">
-        <v>2.42</v>
-      </c>
-      <c r="F28" s="2">
-        <v>4.84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29">
-        <v>0.63</v>
-      </c>
-      <c r="F29">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30">
-        <v>4</v>
-      </c>
-      <c r="B30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30">
-        <v>0.6</v>
-      </c>
-      <c r="F30">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31">
-        <v>10</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31">
-        <v>0.63</v>
-      </c>
-      <c r="F31">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32">
-        <v>0.72</v>
-      </c>
-      <c r="F32">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33">
-        <v>10</v>
-      </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="F33">
-        <v>2.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34">
-        <v>6</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34">
-        <v>0.36</v>
-      </c>
-      <c r="F34">
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="E35">
-        <v>3.79</v>
-      </c>
-      <c r="F35" s="1">
-        <v>7.58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="E36">
-        <v>1.593</v>
-      </c>
-      <c r="F36">
-        <v>19.12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
-        <v>1</v>
-      </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="E38">
-        <v>1.91</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="B39" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
         <v>23</v>
       </c>
-      <c r="E39">
-        <v>0.98</v>
-      </c>
-      <c r="F39" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40">
-        <v>3</v>
-      </c>
-      <c r="B40" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E40">
-        <v>3.58</v>
-      </c>
-      <c r="F40" s="1">
-        <v>10.74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" t="s">
-        <v>83</v>
-      </c>
-      <c r="E41">
-        <v>2.98</v>
-      </c>
-      <c r="F41" s="1">
-        <v>5.96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>86</v>
-      </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>118</v>
+        <v>25</v>
       </c>
       <c r="E42">
-        <v>3.05</v>
-      </c>
-      <c r="F42" s="1">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44">
+        <v>1.593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" t="s">
+        <v>117</v>
+      </c>
+      <c r="E50">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" t="s">
         <v>75</v>
       </c>
-      <c r="C43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="D51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
         <v>64</v>
       </c>
-      <c r="E43">
-        <v>3.05</v>
-      </c>
-      <c r="F43" s="1">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44">
+      <c r="C52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
         <v>10</v>
       </c>
-      <c r="B44" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B54" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" t="s">
         <v>66</v>
       </c>
-      <c r="D44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44">
-        <v>5.5E-2</v>
-      </c>
-      <c r="F44" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45">
+      <c r="E54">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
         <v>10</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" t="s">
         <v>46</v>
       </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45">
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56">
         <v>0.2</v>
       </c>
-      <c r="F45">
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>50</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57">
+        <v>5.7599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>50</v>
+      </c>
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59">
+        <v>5.7599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E60">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62">
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63" t="s">
+        <v>112</v>
+      </c>
+      <c r="E63">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46">
-        <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" t="s">
-        <v>41</v>
-      </c>
-      <c r="E46">
-        <v>5.7599999999999998E-2</v>
-      </c>
-      <c r="F46">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47">
-        <v>4</v>
-      </c>
-      <c r="B47" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F47" s="1">
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48">
-        <v>50</v>
-      </c>
-      <c r="B48" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48">
-        <v>5.7599999999999998E-2</v>
-      </c>
-      <c r="F48">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49">
-        <v>10</v>
-      </c>
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49">
-        <v>0.255</v>
-      </c>
-      <c r="F49" s="1">
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50">
-        <v>8</v>
-      </c>
-      <c r="B50" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" t="s">
-        <v>95</v>
-      </c>
-      <c r="E50">
-        <v>0.47</v>
-      </c>
-      <c r="F50" s="1">
-        <v>3.76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51">
-        <v>0.504</v>
-      </c>
-      <c r="F51">
-        <v>7.06</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" t="s">
-        <v>113</v>
-      </c>
-      <c r="E52">
-        <v>5.89</v>
-      </c>
-      <c r="F52" s="1">
-        <v>5.89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
-        <v>2</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
         <v>125</v>
       </c>
-      <c r="C53" t="s">
-        <v>126</v>
-      </c>
-      <c r="D53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53">
+      <c r="D64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E64">
         <v>0.67</v>
-      </c>
-      <c r="F53" s="2">
-        <v>1.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed PS layout (changed rectifier footprint)
</commit_message>
<xml_diff>
--- a/invoices/Parts_on_hand.xlsx
+++ b/invoices/Parts_on_hand.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="500" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="-38400" yWindow="-2620" windowWidth="38400" windowHeight="21060"/>
   </bookViews>
   <sheets>
     <sheet name="digi_order_4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">digi_order_4!$A$1:$E$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">digi_order_4!$A$1:$E$66</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="173">
   <si>
     <t>Quantity</t>
   </si>
@@ -429,9 +429,6 @@
     <t>CAP CER 1UF 50V X7R RADIAL</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>445-8348-ND</t>
   </si>
   <si>
@@ -486,7 +483,64 @@
     <t>DIODE ZENER 5W 27V DO-15</t>
   </si>
   <si>
-    <t>FOR TEST</t>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>missing 1</t>
+  </si>
+  <si>
+    <t>odered</t>
+  </si>
+  <si>
+    <t>ordered</t>
+  </si>
+  <si>
+    <t>ED2949-ND</t>
+  </si>
+  <si>
+    <t>CONN BARRIER STRIP 6CIRC 8.25MM</t>
+  </si>
+  <si>
+    <t>ED2947-ND</t>
+  </si>
+  <si>
+    <t>CONN BARRIER STRIP 4CIRC 8.25MM</t>
+  </si>
+  <si>
+    <t>A98498-ND</t>
+  </si>
+  <si>
+    <t>CONN BARRIER STRIP 5CIRC .375</t>
+  </si>
+  <si>
+    <t>S4.7KCACT-ND</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1/4W 1% AXIAL</t>
+  </si>
+  <si>
+    <t>445-2637-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 250V X7R RADIAL</t>
+  </si>
+  <si>
+    <t>missing all</t>
+  </si>
+  <si>
+    <t>missing 3</t>
+  </si>
+  <si>
+    <t>missign 9</t>
+  </si>
+  <si>
+    <t>missing 7</t>
+  </si>
+  <si>
+    <t>missing 5</t>
+  </si>
+  <si>
+    <t>mising 5</t>
   </si>
 </sst>
 </file>
@@ -942,7 +996,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="112">
+  <cellStyleXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1055,11 +1109,27 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="112">
+  <cellStyles count="128">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1123,6 +1193,14 @@
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1163,6 +1241,14 @@
     <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1441,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1449,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1464,7 +1550,7 @@
     <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1497,8 +1583,11 @@
       <c r="E2">
         <v>1.68</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1514,8 +1603,11 @@
       <c r="E3">
         <v>2.83</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1531,8 +1623,11 @@
       <c r="E4">
         <v>22.34</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1548,8 +1643,11 @@
       <c r="E5">
         <v>2.91</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1560,44 +1658,56 @@
         <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="E6">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
         <v>146</v>
       </c>
-      <c r="C7" t="s">
-        <v>147</v>
+      <c r="D7" t="s">
+        <v>63</v>
       </c>
       <c r="E7">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" t="s">
         <v>136</v>
       </c>
-      <c r="C8" t="s">
-        <v>137</v>
-      </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="E8">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1613,364 +1723,439 @@
       <c r="E9">
         <v>0.30599999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
         <v>144</v>
       </c>
-      <c r="C10" t="s">
-        <v>145</v>
+      <c r="D10" t="s">
+        <v>117</v>
       </c>
       <c r="E10">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="F11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>0.33700000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
+      <c r="F12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13">
-        <v>0.27800000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="F14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>0.46600000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
+      <c r="F15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="F16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>72</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>73</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>0.23899999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17">
-        <v>0.247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>66</v>
       </c>
       <c r="E18">
+        <v>0.247</v>
+      </c>
+      <c r="F18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19">
         <v>0.64300000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>148</v>
-      </c>
-      <c r="C19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19">
-        <v>1.37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C20" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
       </c>
       <c r="E20">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>1.37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21">
+        <v>0.51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>48</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>49</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
+      <c r="F22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>17</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>19</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>0.17499999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
+      <c r="F23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
+      <c r="F24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>53</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>54</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>0.2316</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
+      <c r="F25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>126</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>127</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>117</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
+      <c r="F26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>95</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>96</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27">
-        <v>9.9000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>22</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>1.28</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>0.4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -1978,407 +2163,479 @@
       <c r="E31">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>0.52</v>
+      </c>
+      <c r="F32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
         <v>1</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" t="s">
         <v>152</v>
       </c>
-      <c r="C32" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" t="s">
-        <v>154</v>
-      </c>
-      <c r="E32">
+      <c r="D33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33">
+      <c r="F33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>89</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>90</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>91</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="E35">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>0.41</v>
+      </c>
+      <c r="F35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36">
+        <v>0.34</v>
+      </c>
+      <c r="F36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>121</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>129</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>2.42</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37">
+      <c r="F37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
         <v>10</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>57</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>58</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>22</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38">
+      <c r="F38" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>8</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>9</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>7</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39">
+      <c r="F39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
         <v>10</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>33</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>34</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>35</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40">
+      <c r="F40" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
         <v>4</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>5</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>7</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41">
+      <c r="F41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
         <v>10</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>20</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>21</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>22</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>0.20200000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42">
+      <c r="F42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
         <v>6</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>23</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>24</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>25</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43">
+      <c r="F43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
         <v>2</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>80</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>81</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>82</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44">
+      <c r="F44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
         <v>12</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>28</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>29</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>30</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>1.593</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45">
+      <c r="F45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
         <v>3</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>55</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>56</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>49</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46">
+      <c r="F46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47">
+        <v>1.91</v>
+      </c>
+      <c r="F47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48">
+        <v>0.98</v>
+      </c>
+      <c r="F48" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49">
+        <v>3.58</v>
+      </c>
+      <c r="F49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50">
+        <v>2.98</v>
+      </c>
+      <c r="F50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
         <v>1</v>
       </c>
-      <c r="B46" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" t="s">
-        <v>116</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" t="s">
         <v>117</v>
-      </c>
-      <c r="E46">
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" t="s">
-        <v>114</v>
-      </c>
-      <c r="D47" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48">
-        <v>3</v>
-      </c>
-      <c r="B48" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48">
-        <v>3.58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49">
-        <v>2</v>
-      </c>
-      <c r="B49" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49">
-        <v>2.98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" t="s">
-        <v>117</v>
-      </c>
-      <c r="E50">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51">
-        <v>2</v>
-      </c>
-      <c r="B51" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" t="s">
-        <v>63</v>
       </c>
       <c r="E51">
         <v>3.05</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52">
+        <v>3.05</v>
+      </c>
+      <c r="F52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
         <v>10</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>64</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>65</v>
-      </c>
-      <c r="D52" t="s">
-        <v>66</v>
-      </c>
-      <c r="E52">
-        <v>5.5E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
-        <v>142</v>
-      </c>
-      <c r="C53" t="s">
-        <v>143</v>
       </c>
       <c r="D53" t="s">
         <v>66</v>
       </c>
       <c r="E53">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C54" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D54" t="s">
         <v>66</v>
       </c>
       <c r="E54">
-        <v>0.255</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>0.36</v>
+      </c>
+      <c r="F54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
         <v>66</v>
@@ -2386,158 +2643,288 @@
       <c r="E55">
         <v>0.255</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>10</v>
       </c>
       <c r="B56" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56">
+        <v>0.255</v>
+      </c>
+      <c r="F56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
         <v>45</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>46</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>22</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57">
+      <c r="F57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
         <v>50</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>41</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>42</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>40</v>
       </c>
-      <c r="E57">
+      <c r="E58">
         <v>5.7599999999999998E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58">
-        <v>4</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" t="s">
-        <v>62</v>
-      </c>
-      <c r="D58" t="s">
-        <v>63</v>
-      </c>
-      <c r="E58">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>163</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="D59" t="s">
         <v>40</v>
       </c>
       <c r="E59">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F60" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>50</v>
+      </c>
+      <c r="B61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61">
         <v>5.7599999999999998E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60">
+      <c r="F61" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
         <v>10</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>87</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C62" t="s">
         <v>88</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D62" t="s">
         <v>66</v>
       </c>
-      <c r="E60">
+      <c r="E62">
         <v>0.255</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61">
+      <c r="F62" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
         <v>8</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>92</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>93</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D63" t="s">
         <v>94</v>
       </c>
-      <c r="E61">
+      <c r="E63">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62">
+      <c r="F63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
         <v>14</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>14</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>15</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D64" t="s">
         <v>16</v>
       </c>
-      <c r="E62">
+      <c r="E64">
         <v>0.504</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63">
+      <c r="F64" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
         <v>1</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>110</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>111</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D65" t="s">
         <v>112</v>
       </c>
-      <c r="E63">
+      <c r="E65">
         <v>5.89</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64">
+      <c r="F65" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
         <v>2</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>124</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>125</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D66" t="s">
         <v>128</v>
       </c>
-      <c r="E64">
+      <c r="E66">
         <v>0.67</v>
+      </c>
+      <c r="F66" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" t="s">
+        <v>158</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67">
+        <v>1.45</v>
+      </c>
+      <c r="F67" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" t="s">
+        <v>132</v>
+      </c>
+      <c r="E68">
+        <v>0.97</v>
+      </c>
+      <c r="F68" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" t="s">
+        <v>162</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69">
+        <v>2.6</v>
+      </c>
+      <c r="F69" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to PS layout
</commit_message>
<xml_diff>
--- a/invoices/Parts_on_hand.xlsx
+++ b/invoices/Parts_on_hand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-2620" windowWidth="38400" windowHeight="21060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="digi_order_4" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="168">
   <si>
     <t>Quantity</t>
   </si>
@@ -486,9 +486,6 @@
     <t>ok</t>
   </si>
   <si>
-    <t>missing 1</t>
-  </si>
-  <si>
     <t>odered</t>
   </si>
   <si>
@@ -525,22 +522,10 @@
     <t>CAP CER 0.1UF 250V X7R RADIAL</t>
   </si>
   <si>
-    <t>missing all</t>
-  </si>
-  <si>
-    <t>missing 3</t>
-  </si>
-  <si>
     <t>missign 9</t>
   </si>
   <si>
     <t>missing 7</t>
-  </si>
-  <si>
-    <t>missing 5</t>
-  </si>
-  <si>
-    <t>mising 5</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1537,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1664,7 +1649,7 @@
         <v>0.4</v>
       </c>
       <c r="F6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1684,7 +1669,7 @@
         <v>0.95</v>
       </c>
       <c r="F7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1704,7 +1689,7 @@
         <v>0.45</v>
       </c>
       <c r="F8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1724,7 +1709,7 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="F9" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1744,7 +1729,7 @@
         <v>0.16</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1752,10 +1737,10 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" t="s">
         <v>165</v>
-      </c>
-      <c r="C11" t="s">
-        <v>166</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -1764,7 +1749,7 @@
         <v>0.31900000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1924,7 +1909,7 @@
         <v>0.64300000000000002</v>
       </c>
       <c r="F19" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1944,7 +1929,7 @@
         <v>1.37</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1964,7 +1949,7 @@
         <v>0.51</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2024,7 +2009,7 @@
         <v>0.41</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2204,7 +2189,7 @@
         <v>0.46</v>
       </c>
       <c r="F33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2344,7 +2329,7 @@
         <v>0.63</v>
       </c>
       <c r="F40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2464,7 +2449,7 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2604,7 +2589,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="F53" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2624,7 +2609,7 @@
         <v>0.36</v>
       </c>
       <c r="F54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2644,7 +2629,7 @@
         <v>0.255</v>
       </c>
       <c r="F55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2664,7 +2649,7 @@
         <v>0.255</v>
       </c>
       <c r="F56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2684,7 +2669,7 @@
         <v>0.2</v>
       </c>
       <c r="F57" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2712,10 +2697,10 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" t="s">
         <v>163</v>
-      </c>
-      <c r="C59" t="s">
-        <v>164</v>
       </c>
       <c r="D59" t="s">
         <v>40</v>
@@ -2724,7 +2709,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
       <c r="F59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2764,7 +2749,7 @@
         <v>5.7599999999999998E-2</v>
       </c>
       <c r="F61" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2824,7 +2809,7 @@
         <v>0.504</v>
       </c>
       <c r="F64" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2872,10 +2857,10 @@
         <v>2</v>
       </c>
       <c r="B67" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" t="s">
         <v>157</v>
-      </c>
-      <c r="C67" t="s">
-        <v>158</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -2884,7 +2869,7 @@
         <v>1.45</v>
       </c>
       <c r="F67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2892,10 +2877,10 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68" t="s">
         <v>159</v>
-      </c>
-      <c r="C68" t="s">
-        <v>160</v>
       </c>
       <c r="D68" t="s">
         <v>132</v>
@@ -2904,7 +2889,7 @@
         <v>0.97</v>
       </c>
       <c r="F68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2912,10 +2897,10 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" t="s">
         <v>161</v>
-      </c>
-      <c r="C69" t="s">
-        <v>162</v>
       </c>
       <c r="D69" t="s">
         <v>82</v>
@@ -2924,7 +2909,7 @@
         <v>2.6</v>
       </c>
       <c r="F69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>